<commit_message>
Adding tests to account for continuous coverage programs
</commit_message>
<xml_diff>
--- a/tests/test_program_calc_progbook.xlsx
+++ b/tests/test_program_calc_progbook.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\atomica\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ECA9DB-4711-47F2-AD03-70B215A57D04}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19725" yWindow="3690" windowWidth="27255" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19725" yWindow="3690" windowWidth="27255" windowHeight="15600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Program targeting" sheetId="1" r:id="rId1"/>
     <sheet name="Spending data" sheetId="2" r:id="rId2"/>
     <sheet name="Program effects" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="41">
   <si>
     <t>Targeted to (populations)</t>
   </si>
@@ -147,12 +146,18 @@
   </si>
   <si>
     <t>people</t>
+  </si>
+  <si>
+    <t>tx_cont</t>
+  </si>
+  <si>
+    <t>TX (continuous)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -254,7 +259,377 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="111">
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFEEEEEE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -935,23 +1310,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -987,23 +1345,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1179,11 +1520,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,84 +1633,132 @@
         <v>30</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="68" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="67" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="66" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="16" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="65" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="64" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="63" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="17" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="62" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="61" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="13" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="60" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="18" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="59" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="58" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="57" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="19" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="56" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="55" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="15" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="54" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:H5 C3:C5" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:H6 C3:C6">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1378,11 +1767,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,129 +2063,262 @@
       </c>
       <c r="F20" s="6"/>
     </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="str">
+        <f>'Program targeting'!$A$6</f>
+        <v>tx_cont</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="6"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="53" priority="13">
+    <cfRule type="expression" dxfId="95" priority="23">
       <formula>COUNTIF(F10:F10,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="14">
+    <cfRule type="expression" dxfId="94" priority="24">
       <formula>AND(COUNTIF(F10:F10,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="51" priority="15">
+    <cfRule type="expression" dxfId="93" priority="25">
       <formula>COUNTIF(F11:F11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="16">
+    <cfRule type="expression" dxfId="92" priority="26">
       <formula>AND(COUNTIF(F11:F11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="49" priority="17">
+    <cfRule type="expression" dxfId="91" priority="27">
       <formula>COUNTIF(F12:F12,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="18">
+    <cfRule type="expression" dxfId="90" priority="28">
       <formula>AND(COUNTIF(F12:F12,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="47" priority="19">
+    <cfRule type="expression" dxfId="89" priority="29">
       <formula>COUNTIF(F13:F13,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="20">
+    <cfRule type="expression" dxfId="88" priority="30">
       <formula>AND(COUNTIF(F13:F13,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="45" priority="21">
+    <cfRule type="expression" dxfId="87" priority="31">
       <formula>COUNTIF(F16:F16,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="22">
+    <cfRule type="expression" dxfId="86" priority="32">
       <formula>AND(COUNTIF(F16:F16,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="43" priority="23">
+    <cfRule type="expression" dxfId="85" priority="33">
       <formula>COUNTIF(F17:F17,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="24">
+    <cfRule type="expression" dxfId="84" priority="34">
       <formula>AND(COUNTIF(F17:F17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="41" priority="25">
+    <cfRule type="expression" dxfId="83" priority="35">
       <formula>COUNTIF(F18:F18,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="26">
+    <cfRule type="expression" dxfId="82" priority="36">
       <formula>AND(COUNTIF(F18:F18,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="39" priority="27">
+    <cfRule type="expression" dxfId="81" priority="37">
       <formula>COUNTIF(F19:F19,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="28">
+    <cfRule type="expression" dxfId="80" priority="38">
       <formula>AND(COUNTIF(F19:F19,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="37" priority="1">
+    <cfRule type="expression" dxfId="79" priority="11">
       <formula>COUNTIF(F2:F2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="2">
+    <cfRule type="expression" dxfId="78" priority="12">
       <formula>AND(COUNTIF(F2:F2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="35" priority="29">
+    <cfRule type="expression" dxfId="77" priority="39">
       <formula>COUNTIF(F20:F20,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="30">
+    <cfRule type="expression" dxfId="76" priority="40">
       <formula>AND(COUNTIF(F20:F20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="33" priority="3">
+    <cfRule type="expression" dxfId="75" priority="13">
       <formula>COUNTIF(F3:F3,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="4">
+    <cfRule type="expression" dxfId="74" priority="14">
       <formula>AND(COUNTIF(F3:F3,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="31" priority="5">
+    <cfRule type="expression" dxfId="73" priority="15">
       <formula>COUNTIF(F4:F4,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="6">
+    <cfRule type="expression" dxfId="72" priority="16">
       <formula>AND(COUNTIF(F4:F4,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="29" priority="7">
+    <cfRule type="expression" dxfId="71" priority="17">
       <formula>COUNTIF(F5:F5,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="8">
+    <cfRule type="expression" dxfId="70" priority="18">
       <formula>AND(COUNTIF(F5:F5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="27" priority="9">
+    <cfRule type="expression" dxfId="69" priority="19">
       <formula>COUNTIF(F6:F6,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="10">
+    <cfRule type="expression" dxfId="68" priority="20">
       <formula>AND(COUNTIF(F6:F6,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="25" priority="11">
+    <cfRule type="expression" dxfId="67" priority="21">
       <formula>COUNTIF(F9:F9,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="12">
+    <cfRule type="expression" dxfId="66" priority="22">
       <formula>AND(COUNTIF(F9:F9,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D9)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="expression" dxfId="41" priority="3">
+      <formula>COUNTIF(F24:F24,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="4">
+      <formula>AND(COUNTIF(F24:F24,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="expression" dxfId="37" priority="5">
+      <formula>COUNTIF(F25:F25,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="6">
+      <formula>AND(COUNTIF(F25:F25,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="expression" dxfId="33" priority="7">
+      <formula>COUNTIF(F26:F26,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="8">
+      <formula>AND(COUNTIF(F26:F26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="expression" dxfId="29" priority="9">
+      <formula>COUNTIF(F27:F27,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="10">
+      <formula>AND(COUNTIF(F27:F27,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="expression" dxfId="25" priority="1">
+      <formula>COUNTIF(F23:F23,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="2">
+      <formula>AND(COUNTIF(F23:F23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(D23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B17 B10" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B17 B10 B24">
       <formula1>"$/person (one-off),$/person/year"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1805,11 +2327,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1819,7 +2341,7 @@
     <col min="7" max="9" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1847,8 +2369,12 @@
         <f>'Program targeting'!$A$5</f>
         <v>art</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="2" t="str">
+        <f>'Program targeting'!$A$6</f>
+        <v>tx_cont</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'Program targeting'!$C$2</f>
         <v>Population 0</v>
@@ -1866,8 +2392,11 @@
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J2" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -1895,8 +2424,12 @@
         <f>'Program targeting'!$A$5</f>
         <v>art</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2" t="str">
+        <f>'Program targeting'!$A$6</f>
+        <v>tx_cont</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'Program targeting'!$C$2</f>
         <v>Population 0</v>
@@ -1914,8 +2447,11 @@
         <v>1</v>
       </c>
       <c r="I5" s="6"/>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J5" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1943,8 +2479,12 @@
         <f>'Program targeting'!$A$5</f>
         <v>art</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2" t="str">
+        <f>'Program targeting'!$A$6</f>
+        <v>tx_cont</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'Program targeting'!$C$2</f>
         <v>Population 0</v>
@@ -1962,34 +2502,35 @@
       <c r="I8" s="6">
         <v>1</v>
       </c>
+      <c r="J8" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="23" priority="7">
+    <cfRule type="expression" dxfId="65" priority="13">
       <formula>COUNTIF(F2:I2,"&lt;&gt;" &amp; "")&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="64" priority="14">
       <formula>AND(COUNTIF(F2:I2,"&lt;&gt;" &amp; "")&lt;2,NOT(ISBLANK(D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="21" priority="15">
+    <cfRule type="expression" dxfId="63" priority="21">
       <formula>COUNTIF(F5:I5,"&lt;&gt;" &amp; "")&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="16">
+    <cfRule type="expression" dxfId="62" priority="22">
       <formula>AND(COUNTIF(F5:I5,"&lt;&gt;" &amp; "")&lt;2,NOT(ISBLANK(D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="19" priority="23">
+    <cfRule type="expression" dxfId="61" priority="29">
       <formula>COUNTIF(F8:I8,"&lt;&gt;" &amp; "")&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="24">
+    <cfRule type="expression" dxfId="60" priority="30">
       <formula>AND(COUNTIF(F8:I8,"&lt;&gt;" &amp; "")&lt;2,NOT(ISBLANK(D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C8 C5" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C8 C5">
       <formula1>"Random,Additive,Nested"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1998,7 +2539,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00000000-000E-0000-0200-000001000000}">
+          <x14:cfRule type="expression" priority="7" id="{00000000-000E-0000-0200-000001000000}">
             <xm:f>AND('Program targeting'!$C$3&lt;&gt;"Y",NOT(ISBLANK(G2)))</xm:f>
             <x14:dxf>
               <fill>
@@ -2008,7 +2549,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="2" id="{00000000-000E-0000-0200-000002000000}">
+          <x14:cfRule type="expression" priority="8" id="{00000000-000E-0000-0200-000002000000}">
             <xm:f>'Program targeting'!$C$3&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
@@ -2037,7 +2578,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="9" id="{00000000-000E-0000-0200-000009000000}">
+          <x14:cfRule type="expression" priority="15" id="{00000000-000E-0000-0200-000009000000}">
             <xm:f>AND('Program targeting'!$C$3&lt;&gt;"Y",NOT(ISBLANK(G5)))</xm:f>
             <x14:dxf>
               <fill>
@@ -2047,7 +2588,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="10" id="{00000000-000E-0000-0200-00000A000000}">
+          <x14:cfRule type="expression" priority="16" id="{00000000-000E-0000-0200-00000A000000}">
             <xm:f>'Program targeting'!$C$3&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
@@ -2076,7 +2617,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="17" id="{00000000-000E-0000-0200-000011000000}">
+          <x14:cfRule type="expression" priority="23" id="{00000000-000E-0000-0200-000011000000}">
             <xm:f>AND('Program targeting'!$C$3&lt;&gt;"Y",NOT(ISBLANK(G8)))</xm:f>
             <x14:dxf>
               <fill>
@@ -2086,7 +2627,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="18" id="{00000000-000E-0000-0200-000012000000}">
+          <x14:cfRule type="expression" priority="24" id="{00000000-000E-0000-0200-000012000000}">
             <xm:f>'Program targeting'!$C$3&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
@@ -2115,7 +2656,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{00000000-000E-0000-0200-000003000000}">
+          <x14:cfRule type="expression" priority="9" id="{00000000-000E-0000-0200-000003000000}">
             <xm:f>AND('Program targeting'!$C$4&lt;&gt;"Y",NOT(ISBLANK(H2)))</xm:f>
             <x14:dxf>
               <fill>
@@ -2125,7 +2666,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="4" id="{00000000-000E-0000-0200-000004000000}">
+          <x14:cfRule type="expression" priority="10" id="{00000000-000E-0000-0200-000004000000}">
             <xm:f>'Program targeting'!$C$4&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
@@ -2154,7 +2695,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="11" id="{00000000-000E-0000-0200-00000B000000}">
+          <x14:cfRule type="expression" priority="17" id="{00000000-000E-0000-0200-00000B000000}">
             <xm:f>AND('Program targeting'!$C$4&lt;&gt;"Y",NOT(ISBLANK(H5)))</xm:f>
             <x14:dxf>
               <fill>
@@ -2164,7 +2705,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="12" id="{00000000-000E-0000-0200-00000C000000}">
+          <x14:cfRule type="expression" priority="18" id="{00000000-000E-0000-0200-00000C000000}">
             <xm:f>'Program targeting'!$C$4&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
@@ -2193,7 +2734,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="19" id="{00000000-000E-0000-0200-000013000000}">
+          <x14:cfRule type="expression" priority="25" id="{00000000-000E-0000-0200-000013000000}">
             <xm:f>AND('Program targeting'!$C$4&lt;&gt;"Y",NOT(ISBLANK(H8)))</xm:f>
             <x14:dxf>
               <fill>
@@ -2203,7 +2744,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="20" id="{00000000-000E-0000-0200-000014000000}">
+          <x14:cfRule type="expression" priority="26" id="{00000000-000E-0000-0200-000014000000}">
             <xm:f>'Program targeting'!$C$4&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
@@ -2232,7 +2773,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{00000000-000E-0000-0200-000005000000}">
+          <x14:cfRule type="expression" priority="11" id="{00000000-000E-0000-0200-000005000000}">
             <xm:f>AND('Program targeting'!$C$5&lt;&gt;"Y",NOT(ISBLANK(I2)))</xm:f>
             <x14:dxf>
               <fill>
@@ -2242,7 +2783,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="6" id="{00000000-000E-0000-0200-000006000000}">
+          <x14:cfRule type="expression" priority="12" id="{00000000-000E-0000-0200-000006000000}">
             <xm:f>'Program targeting'!$C$5&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
@@ -2271,7 +2812,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="13" id="{00000000-000E-0000-0200-00000D000000}">
+          <x14:cfRule type="expression" priority="19" id="{00000000-000E-0000-0200-00000D000000}">
             <xm:f>AND('Program targeting'!$C$5&lt;&gt;"Y",NOT(ISBLANK(I5)))</xm:f>
             <x14:dxf>
               <fill>
@@ -2281,7 +2822,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="14" id="{00000000-000E-0000-0200-00000E000000}">
+          <x14:cfRule type="expression" priority="20" id="{00000000-000E-0000-0200-00000E000000}">
             <xm:f>'Program targeting'!$C$5&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
@@ -2310,7 +2851,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="21" id="{00000000-000E-0000-0200-000015000000}">
+          <x14:cfRule type="expression" priority="27" id="{00000000-000E-0000-0200-000015000000}">
             <xm:f>AND('Program targeting'!$C$5&lt;&gt;"Y",NOT(ISBLANK(I8)))</xm:f>
             <x14:dxf>
               <fill>
@@ -2320,7 +2861,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="22" id="{00000000-000E-0000-0200-000016000000}">
+          <x14:cfRule type="expression" priority="28" id="{00000000-000E-0000-0200-000016000000}">
             <xm:f>'Program targeting'!$C$5&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
@@ -2348,6 +2889,123 @@
           </x14:cfRule>
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{C9EF57C0-A5A7-4371-B041-5120A724A563}">
+            <xm:f>AND('Program targeting'!$C$4&lt;&gt;"Y",NOT(ISBLANK(J2)))</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="lightUp">
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="2" id="{AF92798D-7D8B-489D-93B0-DD39E4A0C1CA}">
+            <xm:f>'Program targeting'!$C$4&lt;&gt;"Y"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="lightUp">
+                  <bgColor rgb="FFEEEEEE"/>
+                </patternFill>
+              </fill>
+              <border>
+                <left style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </left>
+                <right style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </right>
+                <top style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </top>
+                <bottom style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </bottom>
+                <vertical/>
+                <horizontal/>
+              </border>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="3" id="{B6AA4FE6-BAC3-45EA-8F05-544A69AEF538}">
+            <xm:f>AND('Program targeting'!$C$4&lt;&gt;"Y",NOT(ISBLANK(J5)))</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="lightUp">
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="4" id="{AEECA408-5658-46BE-AC48-A686F040CEA7}">
+            <xm:f>'Program targeting'!$C$4&lt;&gt;"Y"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="lightUp">
+                  <bgColor rgb="FFEEEEEE"/>
+                </patternFill>
+              </fill>
+              <border>
+                <left style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </left>
+                <right style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </right>
+                <top style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </top>
+                <bottom style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </bottom>
+                <vertical/>
+                <horizontal/>
+              </border>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="5" id="{E548D9CA-0072-4FE9-9A5B-853FD42498E2}">
+            <xm:f>AND('Program targeting'!$C$4&lt;&gt;"Y",NOT(ISBLANK(J8)))</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="lightUp">
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="6" id="{0337B39E-7D9F-4FB0-BEDE-407367A52CFC}">
+            <xm:f>'Program targeting'!$C$4&lt;&gt;"Y"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="lightUp">
+                  <bgColor rgb="FFEEEEEE"/>
+                </patternFill>
+              </fill>
+              <border>
+                <left style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </left>
+                <right style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </right>
+                <top style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </top>
+                <bottom style="thin">
+                  <color rgb="FFCCCCCC"/>
+                </bottom>
+                <vertical/>
+                <horizontal/>
+              </border>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J8</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>